<commit_message>
Invoice number removed from catering cashbook reports
</commit_message>
<xml_diff>
--- a/src/JCSGYK/AdminBundle/Resources/public/reports/catering_cashbook.xlsx
+++ b/src/JCSGYK/AdminBundle/Resources/public/reports/catering_cashbook.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="15540" yWindow="6520" windowWidth="25600" windowHeight="16060"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>[ca.cim][ca.klub]</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>[catering.month]</t>
-  </si>
-  <si>
-    <t>Számlaszám</t>
-  </si>
-  <si>
-    <t>[catering.invoice_number]</t>
   </si>
 </sst>
 </file>
@@ -794,34 +788,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="3" width="9" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="2" max="2" width="9" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+    <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" ht="43" customHeight="1">
+    <row r="3" spans="1:3" s="8" customFormat="1" ht="43" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -829,29 +821,23 @@
         <v>5</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1">
+    <row r="4" spans="1:3" ht="15" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.8" right="0.2" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>